<commit_message>
created mini-seed.py to test program
</commit_message>
<xml_diff>
--- a/data/mini_seed.xlsx
+++ b/data/mini_seed.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="186">
   <si>
     <t>user_id</t>
   </si>
@@ -490,9 +490,6 @@
     <t>checkin_id</t>
   </si>
   <si>
-    <t>check_in_date</t>
-  </si>
-  <si>
     <t>referral_id</t>
   </si>
   <si>
@@ -581,6 +578,15 @@
   </si>
   <si>
     <t>123@abc.com</t>
+  </si>
+  <si>
+    <t>brr</t>
+  </si>
+  <si>
+    <t>checkin_date</t>
+  </si>
+  <si>
+    <t>brrre</t>
   </si>
 </sst>
 </file>
@@ -1006,7 +1012,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -1390,10 +1396,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1591,74 +1597,74 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:D7"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+    </row>
     <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>179</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="A4">
+        <f>A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <f>A5+1</f>
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <f>A6+1</f>
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>8</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>183</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1"/>
-    <hyperlink ref="C6" r:id="rId2"/>
-    <hyperlink ref="C7" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2487,8 +2493,8 @@
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>2</v>
+      <c r="B3" t="s">
+        <v>183</v>
       </c>
       <c r="C3" t="s">
         <v>140</v>
@@ -2514,7 +2520,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4">
-        <f t="shared" ref="A4:A7" si="0">A3+1</f>
+        <f t="shared" ref="A4:A6" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4">
@@ -2726,8 +2732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2743,7 +2749,7 @@
         <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>153</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3143,19 +3149,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" t="s">
         <v>154</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>155</v>
-      </c>
-      <c r="C1" t="s">
-        <v>156</v>
       </c>
       <c r="D1" t="s">
         <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F1" t="s">
         <v>149</v>
@@ -3257,9 +3263,9 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="L3" workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -3267,7 +3273,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3276,31 +3282,31 @@
         <v>13</v>
       </c>
       <c r="D1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" t="s">
         <v>159</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>160</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>161</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>162</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>163</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>164</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>165</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>166</v>
-      </c>
-      <c r="L1" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -3317,7 +3323,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F2" s="2">
         <v>42964</v>
@@ -3338,7 +3344,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F3" s="2">
         <v>42990</v>
@@ -3347,7 +3353,7 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I3" t="b">
         <v>0</v>
@@ -3371,7 +3377,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F4" s="2">
         <v>43006</v>
@@ -3380,16 +3386,16 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
+        <v>171</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4" t="s">
         <v>172</v>
-      </c>
-      <c r="I4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>4</v>
-      </c>
-      <c r="K4" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -3407,7 +3413,7 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F5" s="2">
         <v>42978</v>
@@ -3428,7 +3434,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F6" s="2">
         <v>43022</v>
@@ -3437,16 +3443,21 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
+        <v>175</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="K6" t="s">
         <v>176</v>
       </c>
-      <c r="I6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>3</v>
-      </c>
-      <c r="K6" t="s">
-        <v>177</v>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="K7" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed mini-seed file and various csv files
</commit_message>
<xml_diff>
--- a/data/mini_seed.xlsx
+++ b/data/mini_seed.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" firstSheet="2" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="184">
   <si>
     <t>user_id</t>
   </si>
@@ -580,13 +580,7 @@
     <t>123@abc.com</t>
   </si>
   <si>
-    <t>brr</t>
-  </si>
-  <si>
     <t>checkin_date</t>
-  </si>
-  <si>
-    <t>brrre</t>
   </si>
 </sst>
 </file>
@@ -1599,7 +1593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
@@ -1819,7 +1813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -2425,7 +2419,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2493,8 +2487,8 @@
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>183</v>
+      <c r="B3">
+        <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>140</v>
@@ -2749,7 +2743,7 @@
         <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3263,10 +3257,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView topLeftCell="L3" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3453,11 +3447,6 @@
       </c>
       <c r="K6" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="K7" t="s">
-        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>